<commit_message>
Alterações no login e token
</commit_message>
<xml_diff>
--- a/SpMedGroup-Tabelas.xlsx
+++ b/SpMedGroup-Tabelas.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\47575406808\Desktop\Sprint 1\SPMedGroup\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\47575406808\Desktop\Sprint2\Senai.SpMedGroup.Manha\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="120">
   <si>
     <t>Usuarios</t>
   </si>
@@ -225,15 +225,6 @@
   </si>
   <si>
     <t>65463-SP</t>
-  </si>
-  <si>
-    <t>Ricardo Lemos</t>
-  </si>
-  <si>
-    <t>Roberto Possarle</t>
-  </si>
-  <si>
-    <t>Helena Strada</t>
   </si>
   <si>
     <t>EMAIL</t>
@@ -1217,7 +1208,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E8"/>
+      <selection activeCell="A9" sqref="A9:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1255,7 +1246,7 @@
         <v>55</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E2" s="14">
         <v>30602</v>
@@ -1272,7 +1263,7 @@
         <v>56</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E3" s="14">
         <v>37095</v>
@@ -1289,7 +1280,7 @@
         <v>57</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E4" s="14">
         <v>28773</v>
@@ -1306,7 +1297,7 @@
         <v>58</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E5" s="14">
         <v>31333</v>
@@ -1323,7 +1314,7 @@
         <v>59</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E6" s="14">
         <v>27633</v>
@@ -1340,7 +1331,7 @@
         <v>60</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E7" s="14">
         <v>26379</v>
@@ -1357,7 +1348,7 @@
         <v>61</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E8" s="14">
         <v>43164</v>
@@ -1382,7 +1373,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1408,15 +1399,15 @@
         <v>40</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="16" t="s">
-        <v>65</v>
+      <c r="B2" s="16">
+        <v>31</v>
       </c>
       <c r="C2" s="16">
         <v>2</v>
@@ -1425,15 +1416,15 @@
         <v>1</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="16" t="s">
-        <v>66</v>
+      <c r="B3" s="16">
+        <v>30</v>
       </c>
       <c r="C3" s="16">
         <v>17</v>
@@ -1442,15 +1433,15 @@
         <v>1</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="B4" s="16" t="s">
-        <v>67</v>
+      <c r="B4" s="16">
+        <v>29</v>
       </c>
       <c r="C4" s="17">
         <v>16</v>
@@ -1459,7 +1450,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1491,36 +1482,36 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C1" t="s">
         <v>28</v>
       </c>
       <c r="D1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="B2" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="C2" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>75</v>
-      </c>
       <c r="E2" s="22" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1548,19 +1539,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D1" t="s">
         <v>106</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>107</v>
-      </c>
-      <c r="C1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D1" t="s">
-        <v>109</v>
-      </c>
-      <c r="E1" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -1678,7 +1669,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
@@ -1688,17 +1679,17 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -1724,19 +1715,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" t="s">
         <v>78</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>79</v>
-      </c>
-      <c r="C1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E1" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -1747,13 +1738,13 @@
         <v>94839859000</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -1764,13 +1755,13 @@
         <v>73556944057</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -1781,13 +1772,13 @@
         <v>16839338002</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E4" s="21" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -1798,13 +1789,13 @@
         <v>14332654765</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E5" s="21" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1815,13 +1806,13 @@
         <v>91305348010</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -1832,13 +1823,13 @@
         <v>79799299004</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -1849,13 +1840,13 @@
         <v>13771913039</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E8" s="21" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>